<commit_message>
fixing main-loop inclusion of indicators
</commit_message>
<xml_diff>
--- a/EduAnalysisTool/input_tool/edu_table_helper_FR_BFA.xlsx
+++ b/EduAnalysisTool/input_tool/edu_table_helper_FR_BFA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNA_2024_EduAnalysis/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{12BE1669-350D-4A48-9691-8F4FC8C1B4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7444DAC6-76F3-4712-B44E-EF8A16C13353}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{12BE1669-350D-4A48-9691-8F4FC8C1B4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B4C4565-6F90-4A12-971A-1DA3FC44262B}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" activeTab="8" xr2:uid="{AD85D784-B454-4039-8455-21301024D336}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" firstSheet="4" activeTab="8" xr2:uid="{AD85D784-B454-4039-8455-21301024D336}"/>
   </bookViews>
   <sheets>
     <sheet name="access" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>out_of_school</t>
   </si>
   <si>
-    <t>% d'enfants en âge scolaire ayant fréquenté l'école ou un programme d'éducation pré-primaire en 2023-2024</t>
-  </si>
-  <si>
     <t>Interruption</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Non-scolarisation</t>
   </si>
   <si>
-    <t>% d'enfants en âge scolaire n'ayant pas fréquenté l'école ou un programme d'éducation pré-primaire à n'importe quel moment de l'année scolaire 2023-2024</t>
-  </si>
-  <si>
     <t>Barrières</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
     <t>% d'enfants en âge scolaire dont l'école a été occupée par des déplacés</t>
   </si>
   <si>
-    <t>% d'enfants d'âge scolaire dont l'éducation a été interrompue par l'occupation de l'école par les forces armées</t>
-  </si>
-  <si>
     <t>non_formal</t>
   </si>
   <si>
@@ -181,18 +172,6 @@
     <t>Non-formel</t>
   </si>
   <si>
-    <t>Absence d'école accessible dans la communauté</t>
-  </si>
-  <si>
-    <t>Impossibilité d'assumer les coûts les frais de scolarité</t>
-  </si>
-  <si>
-    <t>Manque d’intérêt/L’éducation n’est pas une priorité pour l’enfant ou le ménage</t>
-  </si>
-  <si>
-    <t>L'enfant participe à des activités génératrices de revenus en dehors du ménage</t>
-  </si>
-  <si>
     <t>L'enfant n'est pas considéré comme l'âge d'aller à l'école</t>
   </si>
   <si>
@@ -208,18 +187,12 @@
     <t>Cours d'alphabétisation</t>
   </si>
   <si>
-    <t>Cours Stratégie de Scolarisation Accélérée par Passerelles</t>
-  </si>
-  <si>
     <t>Cours de rattrapage</t>
   </si>
   <si>
     <t>Formation technique et d'apprentissage des jeunes</t>
   </si>
   <si>
-    <t>Enseignement coranique</t>
-  </si>
-  <si>
     <t>Cours à la télévision</t>
   </si>
   <si>
@@ -244,14 +217,41 @@
     <t>% d'enfants accédant à l'éducation en dehors des écoles formelles</t>
   </si>
   <si>
-    <t>type_radio</t>
+    <t>% d'enfants en âge scolaire ayant fréquenté l'école ou un programme d'éducation pré-primaire en 2024-2025</t>
+  </si>
+  <si>
+    <t>% d'enfants en âge scolaire n'ayant pas fréquenté l'école ou un programme d'éducation pré-primaire à n'importe quel moment de l'année scolaire 2024-2025</t>
+  </si>
+  <si>
+    <t>% d'enfants en âge scolaire dont l'éducation a été perturbée par des attaques directes contre l'éducation</t>
+  </si>
+  <si>
+    <t>L’éducation n’est pas une priorité pour l’enfant ou le ménage</t>
+  </si>
+  <si>
+    <t>L’école a été fermée en raison de dommages, de catastrophes naturelles, d'insecurité</t>
+  </si>
+  <si>
+    <t>Impossibilité d'assumer les frais de scolarité , inscription</t>
+  </si>
+  <si>
+    <t>Manque d’intérêt pour l'éducation formelle</t>
+  </si>
+  <si>
+    <t>Cours Stratégie de Scolarisation Accélérée par Passerelless, SSAP</t>
+  </si>
+  <si>
+    <t>Cours à la radio</t>
+  </si>
+  <si>
+    <t>Enseignement coranique, école franco-arabe non prise en compte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,8 +291,19 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,8 +316,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -314,12 +331,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -329,6 +361,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -667,18 +705,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0B085A-F222-4D02-94C7-458C197FFE9F}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="E1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
     <col min="6" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,58 +739,58 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.75">
+      <c r="G5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G7" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -764,20 +802,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08680CC-21CB-4C65-AC6D-F24FF5598654}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
     <col min="6" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -800,43 +838,43 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.8">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.8">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.8">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -848,16 +886,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39444B71-EEA9-4171-A7FB-692AC9A3C4DA}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="7" width="28.85546875" customWidth="1"/>
+    <col min="1" max="7" width="28.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -880,59 +918,59 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="G5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="G6" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="G7" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -946,18 +984,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,40 +1018,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1026,18 +1064,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1060,40 +1098,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1106,18 +1144,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1140,40 +1178,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1186,18 +1224,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1220,37 +1258,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1263,18 +1301,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1297,37 +1335,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1340,17 +1378,17 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" customWidth="1"/>
     <col min="6" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1373,78 +1411,78 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G7" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="3" t="s">
-        <v>61</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G8" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G9" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G10" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="G11" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>